<commit_message>
add necessary information in quaternary for runtime stack
</commit_message>
<xml_diff>
--- a/DesignDocs/E1 四元式设计.xlsx
+++ b/DesignDocs/E1 四元式设计.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="101">
   <si>
     <t>四元式设计</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -272,14 +272,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>函数/过程调用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CALL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>传递参数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -303,10 +295,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BEGIN PROC/FUNC at TokenTable[PROC_FUNC_INDEX]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PARA_NUM</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -347,10 +335,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Call Procedure or Function with PARANUM parameters</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>这里的PARA_NUM一定要有，因为后面的SETP可能不是连续的</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -376,6 +360,60 @@
   </si>
   <si>
     <t>WRITE(DST[OFFSET])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FUNC_INDEX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PROC_INDEX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Call Procedure with PARANUM parameters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Call Function with PARANUM parameters</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>过程调用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>函数调用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PROC_CALL</t>
+  </si>
+  <si>
+    <t>FUNC_CALL</t>
+  </si>
+  <si>
+    <t>寄存器转储</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STORE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DST=[EAX]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TEMPNUM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BEGIN PROC/FUNC at TokenTable[PROC_FUNC_INDEX], with TEMPNUM temporary variables</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -731,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -742,6 +780,7 @@
     <col min="1" max="1" width="5.375" customWidth="1"/>
     <col min="2" max="2" width="14.5" customWidth="1"/>
     <col min="4" max="4" width="10.625" customWidth="1"/>
+    <col min="5" max="5" width="9.875" customWidth="1"/>
     <col min="6" max="6" width="17.25" customWidth="1"/>
     <col min="7" max="7" width="51.25" customWidth="1"/>
   </cols>
@@ -776,24 +815,24 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" t="s">
         <v>74</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" t="s">
         <v>75</v>
-      </c>
-      <c r="E3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -922,51 +961,45 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="2" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="2"/>
+      <c r="B10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>40</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>37</v>
-      </c>
-      <c r="F11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="2"/>
-      <c r="B12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" t="s">
-        <v>19</v>
       </c>
       <c r="F12" t="s">
         <v>38</v>
       </c>
       <c r="G12" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="2"/>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" t="s">
         <v>17</v>
@@ -978,16 +1011,16 @@
         <v>38</v>
       </c>
       <c r="G13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="2"/>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" t="s">
         <v>17</v>
@@ -999,16 +1032,16 @@
         <v>38</v>
       </c>
       <c r="G14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="2"/>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
         <v>17</v>
@@ -1020,16 +1053,16 @@
         <v>38</v>
       </c>
       <c r="G15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="2"/>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
         <v>17</v>
@@ -1041,16 +1074,16 @@
         <v>38</v>
       </c>
       <c r="G16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" s="2"/>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
         <v>17</v>
@@ -1062,164 +1095,209 @@
         <v>38</v>
       </c>
       <c r="G17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" s="2"/>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>52</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="F18" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="G18" t="s">
-        <v>83</v>
-      </c>
-      <c r="H18" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="2"/>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>93</v>
+      </c>
+      <c r="E19" t="s">
+        <v>70</v>
       </c>
       <c r="F19" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="G19" t="s">
         <v>89</v>
+      </c>
+      <c r="H19" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" s="2"/>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C20" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E20" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F20" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="G20" t="s">
         <v>90</v>
+      </c>
+      <c r="H20" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" s="2"/>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="F21" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="G21" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" s="2"/>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="C22" t="s">
+        <v>84</v>
+      </c>
+      <c r="E22" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" t="s">
+        <v>73</v>
+      </c>
+      <c r="G22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A23" s="2"/>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A24" s="2"/>
+      <c r="B24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>99</v>
+      </c>
+      <c r="F26" t="s">
         <v>68</v>
       </c>
-      <c r="E22" t="s">
-        <v>79</v>
-      </c>
-      <c r="F22" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="F24" t="s">
-        <v>70</v>
-      </c>
-      <c r="G24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A25" s="2"/>
-      <c r="B25" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25" t="s">
-        <v>69</v>
-      </c>
-      <c r="G25" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A26" s="2"/>
-      <c r="B26" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" t="s">
-        <v>62</v>
-      </c>
       <c r="G26" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27" s="2"/>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A28" s="2"/>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A30" s="1"/>
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A32" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A11:A22"/>
+    <mergeCell ref="A12:A24"/>
     <mergeCell ref="B1:G1"/>
-    <mergeCell ref="A24:A29"/>
-    <mergeCell ref="A3:A9"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="A3:A10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update with design docs
</commit_message>
<xml_diff>
--- a/DesignDocs/E1 四元式设计.xlsx
+++ b/DesignDocs/E1 四元式设计.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="14805" windowHeight="7980" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="101">
   <si>
     <t>四元式设计</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -307,22 +307,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OFFSET</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DST[OFFSET]=-DST[OFFSET]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OFFSET</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PUSH DST[OFFSET]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -335,10 +323,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>这里的PARA_NUM一定要有，因为后面的SETP可能不是连续的</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>读语句</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -401,10 +385,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DST=[EAX]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -414,6 +394,26 @@
   </si>
   <si>
     <t>BEGIN PROC/FUNC at TokenTable[PROC_FUNC_INDEX], with TEMPNUM temporary variables</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>这里的PARA_NUM一定要有，因为在调用完后要调整栈指针</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Call Function</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Call Procedure </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TMP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TMP=[EAX]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -769,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -782,7 +782,7 @@
     <col min="4" max="4" width="10.625" customWidth="1"/>
     <col min="5" max="5" width="9.875" customWidth="1"/>
     <col min="6" max="6" width="17.25" customWidth="1"/>
-    <col min="7" max="7" width="51.25" customWidth="1"/>
+    <col min="7" max="7" width="41.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
@@ -826,13 +826,13 @@
         <v>72</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
         <v>73</v>
-      </c>
-      <c r="G3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -964,16 +964,16 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F10" t="s">
-        <v>97</v>
+        <v>20</v>
       </c>
       <c r="G10" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
@@ -1077,7 +1077,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="2"/>
       <c r="B17" t="s">
         <v>42</v>
@@ -1098,7 +1098,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="2"/>
       <c r="B18" t="s">
         <v>49</v>
@@ -1119,100 +1119,88 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="2"/>
       <c r="B19" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C19" t="s">
-        <v>93</v>
-      </c>
-      <c r="E19" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="F19" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G19" t="s">
-        <v>89</v>
-      </c>
-      <c r="H19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" s="2"/>
       <c r="B20" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="F20" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G20" t="s">
-        <v>90</v>
-      </c>
-      <c r="H20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21" s="2"/>
       <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" t="s">
         <v>81</v>
       </c>
-      <c r="C21" t="s">
-        <v>83</v>
-      </c>
-      <c r="F21" t="s">
-        <v>73</v>
-      </c>
-      <c r="G21" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" s="2"/>
       <c r="B22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" t="s">
         <v>82</v>
       </c>
-      <c r="C22" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" t="s">
-        <v>74</v>
-      </c>
-      <c r="F22" t="s">
-        <v>73</v>
-      </c>
-      <c r="G22" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23" s="2"/>
       <c r="B23" t="s">
         <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" t="s">
         <v>74</v>
       </c>
-      <c r="F23" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24" s="2"/>
       <c r="B24" t="s">
         <v>65</v>
@@ -1221,16 +1209,16 @@
         <v>66</v>
       </c>
       <c r="E24" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="F24" t="s">
         <v>20</v>
       </c>
       <c r="G24" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>3</v>
       </c>
@@ -1241,16 +1229,16 @@
         <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="F26" t="s">
         <v>68</v>
       </c>
       <c r="G26" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" s="2"/>
       <c r="B27" t="s">
         <v>60</v>
@@ -1265,7 +1253,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28" s="2"/>
       <c r="B28" t="s">
         <v>61</v>
@@ -1280,16 +1268,16 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
     </row>
   </sheetData>
@@ -1307,10 +1295,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1318,96 +1306,524 @@
     <col min="1" max="1" width="5.375" customWidth="1"/>
     <col min="2" max="2" width="14.5" customWidth="1"/>
     <col min="4" max="4" width="10.625" customWidth="1"/>
+    <col min="5" max="5" width="9.875" customWidth="1"/>
     <col min="6" max="6" width="17.25" customWidth="1"/>
-    <col min="7" max="7" width="51.25" customWidth="1"/>
+    <col min="7" max="7" width="41.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B1" s="3"/>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="2"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2"/>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2"/>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2"/>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="2"/>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2"/>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="2"/>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="2"/>
+      <c r="B10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G10" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="2"/>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="2"/>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="2"/>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" s="2"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B19" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" t="s">
+        <v>85</v>
+      </c>
+      <c r="H19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" s="2"/>
-    </row>
-    <row r="22" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" t="s">
+        <v>83</v>
+      </c>
+      <c r="G20" t="s">
+        <v>86</v>
+      </c>
+      <c r="H20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A21" s="2"/>
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" s="2"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A24" s="2"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A25" s="2"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A26" s="2"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>94</v>
+      </c>
+      <c r="F26" t="s">
+        <v>68</v>
+      </c>
+      <c r="G26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27" s="2"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A28" s="1"/>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A28" s="2"/>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A32" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:G1"/>
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="A11:A20"/>
-    <mergeCell ref="A22:A27"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="A12:A24"/>
+    <mergeCell ref="A26:A31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
function return value implemented
</commit_message>
<xml_diff>
--- a/DesignDocs/E1 四元式设计.xlsx
+++ b/DesignDocs/E1 四元式设计.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="106">
   <si>
     <t>四元式设计</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -409,11 +409,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TMP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TMP=[EAX]</t>
+    <t>DST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DST=[EAX]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRC1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRC1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DST=-SRC1[OFFSET]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DST[OFFSET]=SRC1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -421,7 +441,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,6 +454,13 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -457,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
@@ -468,6 +495,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1295,10 +1323,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1351,14 +1379,17 @@
       <c r="C3" t="s">
         <v>72</v>
       </c>
+      <c r="D3" t="s">
+        <v>103</v>
+      </c>
       <c r="E3" t="s">
         <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="G3" t="s">
-        <v>73</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -1454,7 +1485,7 @@
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="E8" t="s">
         <v>26</v>
@@ -1475,7 +1506,7 @@
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>102</v>
       </c>
       <c r="E9" t="s">
         <v>26</v>
@@ -1484,21 +1515,21 @@
         <v>20</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="4" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1648,40 +1679,37 @@
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="2"/>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="C19" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E19" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="F19" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="G19" t="s">
-        <v>85</v>
-      </c>
-      <c r="H19" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" s="2"/>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E20" t="s">
         <v>70</v>
       </c>
       <c r="F20" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H20" t="s">
         <v>96</v>
@@ -1690,25 +1718,31 @@
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" s="2"/>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>90</v>
+      </c>
+      <c r="E21" t="s">
+        <v>70</v>
       </c>
       <c r="F21" t="s">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="G21" t="s">
-        <v>81</v>
+        <v>86</v>
+      </c>
+      <c r="H21" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" s="2"/>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="E22" t="s">
         <v>26</v>
@@ -1717,97 +1751,106 @@
         <v>20</v>
       </c>
       <c r="G22" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23" s="2"/>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
-      </c>
-      <c r="E23" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="F23" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="G23" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A24" s="2"/>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A25" s="2"/>
+      <c r="B25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25" t="s">
         <v>26</v>
       </c>
-      <c r="F24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="2" t="s">
+      <c r="F25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>59</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>4</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>94</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F27" t="s">
         <v>68</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G27" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A27" s="2"/>
-      <c r="B27" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" t="s">
-        <v>67</v>
-      </c>
-      <c r="G27" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A28" s="2"/>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="F28" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="G28" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A29" s="2"/>
+      <c r="B29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" t="s">
+        <v>62</v>
+      </c>
+      <c r="G29" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A30" s="2"/>
@@ -1816,17 +1859,21 @@
       <c r="A31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A32" s="1"/>
+      <c r="A32" s="2"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="A3:A10"/>
-    <mergeCell ref="A12:A24"/>
-    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="A12:A25"/>
+    <mergeCell ref="A27:A32"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
all function completed at 20:23 2/2 2016
</commit_message>
<xml_diff>
--- a/DesignDocs/E1 四元式设计.xlsx
+++ b/DesignDocs/E1 四元式设计.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="107">
   <si>
     <t>四元式设计</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -434,6 +434,10 @@
   </si>
   <si>
     <t>DST[OFFSET]=SRC1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>函数调用</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -464,12 +468,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -484,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
@@ -493,9 +503,13 @@
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -814,14 +828,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
@@ -844,7 +858,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -864,7 +878,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2"/>
+      <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>22</v>
       </c>
@@ -885,7 +899,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="2"/>
+      <c r="A5" s="3"/>
       <c r="B5" t="s">
         <v>23</v>
       </c>
@@ -906,7 +920,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="2"/>
+      <c r="A6" s="3"/>
       <c r="B6" t="s">
         <v>24</v>
       </c>
@@ -927,7 +941,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="2"/>
+      <c r="A7" s="3"/>
       <c r="B7" t="s">
         <v>25</v>
       </c>
@@ -948,7 +962,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="2"/>
+      <c r="A8" s="3"/>
       <c r="B8" t="s">
         <v>36</v>
       </c>
@@ -969,7 +983,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="2"/>
+      <c r="A9" s="3"/>
       <c r="B9" t="s">
         <v>35</v>
       </c>
@@ -990,7 +1004,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="2"/>
+      <c r="A10" s="3"/>
       <c r="B10" t="s">
         <v>91</v>
       </c>
@@ -1005,7 +1019,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B12" t="s">
@@ -1022,7 +1036,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="2"/>
+      <c r="A13" s="3"/>
       <c r="B13" t="s">
         <v>43</v>
       </c>
@@ -1043,7 +1057,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="2"/>
+      <c r="A14" s="3"/>
       <c r="B14" t="s">
         <v>44</v>
       </c>
@@ -1064,7 +1078,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="2"/>
+      <c r="A15" s="3"/>
       <c r="B15" t="s">
         <v>41</v>
       </c>
@@ -1085,7 +1099,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="2"/>
+      <c r="A16" s="3"/>
       <c r="B16" t="s">
         <v>48</v>
       </c>
@@ -1106,7 +1120,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A17" s="2"/>
+      <c r="A17" s="3"/>
       <c r="B17" t="s">
         <v>42</v>
       </c>
@@ -1127,7 +1141,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A18" s="2"/>
+      <c r="A18" s="3"/>
       <c r="B18" t="s">
         <v>49</v>
       </c>
@@ -1148,7 +1162,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A19" s="2"/>
+      <c r="A19" s="3"/>
       <c r="B19" t="s">
         <v>87</v>
       </c>
@@ -1163,7 +1177,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A20" s="2"/>
+      <c r="A20" s="3"/>
       <c r="B20" t="s">
         <v>88</v>
       </c>
@@ -1178,7 +1192,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A21" s="2"/>
+      <c r="A21" s="3"/>
       <c r="B21" t="s">
         <v>77</v>
       </c>
@@ -1193,7 +1207,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A22" s="2"/>
+      <c r="A22" s="3"/>
       <c r="B22" t="s">
         <v>78</v>
       </c>
@@ -1211,7 +1225,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" s="2"/>
+      <c r="A23" s="3"/>
       <c r="B23" t="s">
         <v>64</v>
       </c>
@@ -1229,7 +1243,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" s="2"/>
+      <c r="A24" s="3"/>
       <c r="B24" t="s">
         <v>65</v>
       </c>
@@ -1247,7 +1261,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B26" t="s">
@@ -1267,7 +1281,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A27" s="2"/>
+      <c r="A27" s="3"/>
       <c r="B27" t="s">
         <v>60</v>
       </c>
@@ -1282,7 +1296,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A28" s="2"/>
+      <c r="A28" s="3"/>
       <c r="B28" t="s">
         <v>61</v>
       </c>
@@ -1297,13 +1311,13 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A29" s="2"/>
+      <c r="A29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A30" s="2"/>
+      <c r="A30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A31" s="2"/>
+      <c r="A31" s="3"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
@@ -1323,10 +1337,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1340,14 +1354,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
@@ -1370,7 +1384,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -1393,7 +1407,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2"/>
+      <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>22</v>
       </c>
@@ -1414,7 +1428,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="2"/>
+      <c r="A5" s="3"/>
       <c r="B5" t="s">
         <v>23</v>
       </c>
@@ -1435,7 +1449,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="2"/>
+      <c r="A6" s="3"/>
       <c r="B6" t="s">
         <v>24</v>
       </c>
@@ -1456,7 +1470,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="2"/>
+      <c r="A7" s="3"/>
       <c r="B7" t="s">
         <v>25</v>
       </c>
@@ -1477,7 +1491,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="2"/>
+      <c r="A8" s="3"/>
       <c r="B8" t="s">
         <v>36</v>
       </c>
@@ -1498,7 +1512,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="2"/>
+      <c r="A9" s="3"/>
       <c r="B9" t="s">
         <v>35</v>
       </c>
@@ -1518,23 +1532,23 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="2"/>
-      <c r="B10" s="4" t="s">
+    <row r="10" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="3"/>
+      <c r="B10" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B12" t="s">
@@ -1551,7 +1565,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="2"/>
+      <c r="A13" s="3"/>
       <c r="B13" t="s">
         <v>43</v>
       </c>
@@ -1572,7 +1586,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="2"/>
+      <c r="A14" s="3"/>
       <c r="B14" t="s">
         <v>44</v>
       </c>
@@ -1593,7 +1607,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="2"/>
+      <c r="A15" s="3"/>
       <c r="B15" t="s">
         <v>41</v>
       </c>
@@ -1614,7 +1628,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="2"/>
+      <c r="A16" s="3"/>
       <c r="B16" t="s">
         <v>48</v>
       </c>
@@ -1635,7 +1649,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A17" s="2"/>
+      <c r="A17" s="3"/>
       <c r="B17" t="s">
         <v>42</v>
       </c>
@@ -1656,7 +1670,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A18" s="2"/>
+      <c r="A18" s="3"/>
       <c r="B18" t="s">
         <v>49</v>
       </c>
@@ -1677,199 +1691,206 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A19" s="2"/>
+      <c r="A19" s="3"/>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
-      </c>
-      <c r="E19" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="F19" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="G19" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" s="2"/>
-      <c r="B20" t="s">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A21" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A22" s="3"/>
+      <c r="B22" t="s">
         <v>87</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C22" t="s">
         <v>89</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E22" t="s">
         <v>70</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F22" t="s">
         <v>84</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G22" t="s">
         <v>85</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H22" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A21" s="2"/>
-      <c r="B21" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A23" s="3"/>
+      <c r="B23" t="s">
         <v>88</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" t="s">
         <v>90</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E23" t="s">
         <v>70</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F23" t="s">
         <v>83</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G23" t="s">
         <v>86</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H23" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A22" s="2"/>
-      <c r="B22" t="s">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A24" s="3"/>
+      <c r="B24" t="s">
         <v>65</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C24" t="s">
         <v>66</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E24" t="s">
         <v>26</v>
       </c>
-      <c r="F22" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="F24" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A23" s="2"/>
-      <c r="B23" t="s">
+    <row r="25" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="3"/>
+      <c r="B25" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C25" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F25" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G25" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A24" s="2"/>
-      <c r="B24" t="s">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A26" s="3"/>
+      <c r="B26" t="s">
         <v>77</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" t="s">
         <v>79</v>
       </c>
-      <c r="F24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="F26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A25" s="2"/>
-      <c r="B25" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A27" s="3"/>
+      <c r="B27" t="s">
         <v>78</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C27" t="s">
         <v>80</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E27" t="s">
         <v>26</v>
       </c>
-      <c r="F25" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" t="s">
+      <c r="F27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="2" t="s">
+    <row r="28" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="29" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B27" t="s">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A30" s="3"/>
+      <c r="B30" t="s">
         <v>59</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C30" t="s">
         <v>4</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E30" t="s">
         <v>94</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F30" t="s">
         <v>68</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G30" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A28" s="2"/>
-      <c r="B28" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A31" s="3"/>
+      <c r="B31" t="s">
         <v>60</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C31" t="s">
         <v>5</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F31" t="s">
         <v>67</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G31" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A29" s="2"/>
-      <c r="B29" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F29" t="s">
-        <v>62</v>
-      </c>
-      <c r="G29" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A30" s="2"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A31" s="2"/>
-    </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A32" s="2"/>
+      <c r="A32" s="3"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A33" s="1"/>
+      <c r="A33" s="3"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
+    <mergeCell ref="A29:A34"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="A3:A10"/>
-    <mergeCell ref="A12:A25"/>
-    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="A21:A27"/>
+    <mergeCell ref="A12:A19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
optimize the compare instruction generating process
</commit_message>
<xml_diff>
--- a/DesignDocs/E1 四元式设计.xlsx
+++ b/DesignDocs/E1 四元式设计.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="112">
   <si>
     <t>四元式设计</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -438,6 +438,26 @@
   </si>
   <si>
     <t>函数调用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>传递引用参数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SETREFP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OFFSET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PUSH DST[OFFSET].addr</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -502,14 +522,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -828,14 +848,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
@@ -858,7 +878,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -878,7 +898,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="3"/>
+      <c r="A4" s="5"/>
       <c r="B4" t="s">
         <v>22</v>
       </c>
@@ -899,7 +919,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="3"/>
+      <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>23</v>
       </c>
@@ -920,7 +940,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="3"/>
+      <c r="A6" s="5"/>
       <c r="B6" t="s">
         <v>24</v>
       </c>
@@ -941,7 +961,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="3"/>
+      <c r="A7" s="5"/>
       <c r="B7" t="s">
         <v>25</v>
       </c>
@@ -962,7 +982,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="3"/>
+      <c r="A8" s="5"/>
       <c r="B8" t="s">
         <v>36</v>
       </c>
@@ -983,7 +1003,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="3"/>
+      <c r="A9" s="5"/>
       <c r="B9" t="s">
         <v>35</v>
       </c>
@@ -1004,7 +1024,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A10" s="3"/>
+      <c r="A10" s="5"/>
       <c r="B10" t="s">
         <v>91</v>
       </c>
@@ -1019,7 +1039,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B12" t="s">
@@ -1036,7 +1056,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="3"/>
+      <c r="A13" s="5"/>
       <c r="B13" t="s">
         <v>43</v>
       </c>
@@ -1057,7 +1077,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="3"/>
+      <c r="A14" s="5"/>
       <c r="B14" t="s">
         <v>44</v>
       </c>
@@ -1078,7 +1098,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="3"/>
+      <c r="A15" s="5"/>
       <c r="B15" t="s">
         <v>41</v>
       </c>
@@ -1099,7 +1119,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="3"/>
+      <c r="A16" s="5"/>
       <c r="B16" t="s">
         <v>48</v>
       </c>
@@ -1120,7 +1140,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A17" s="3"/>
+      <c r="A17" s="5"/>
       <c r="B17" t="s">
         <v>42</v>
       </c>
@@ -1141,7 +1161,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A18" s="3"/>
+      <c r="A18" s="5"/>
       <c r="B18" t="s">
         <v>49</v>
       </c>
@@ -1162,7 +1182,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A19" s="3"/>
+      <c r="A19" s="5"/>
       <c r="B19" t="s">
         <v>87</v>
       </c>
@@ -1177,7 +1197,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A20" s="3"/>
+      <c r="A20" s="5"/>
       <c r="B20" t="s">
         <v>88</v>
       </c>
@@ -1192,7 +1212,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A21" s="3"/>
+      <c r="A21" s="5"/>
       <c r="B21" t="s">
         <v>77</v>
       </c>
@@ -1207,7 +1227,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A22" s="3"/>
+      <c r="A22" s="5"/>
       <c r="B22" t="s">
         <v>78</v>
       </c>
@@ -1225,7 +1245,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" s="3"/>
+      <c r="A23" s="5"/>
       <c r="B23" t="s">
         <v>64</v>
       </c>
@@ -1243,7 +1263,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" s="3"/>
+      <c r="A24" s="5"/>
       <c r="B24" t="s">
         <v>65</v>
       </c>
@@ -1261,7 +1281,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B26" t="s">
@@ -1281,7 +1301,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A27" s="3"/>
+      <c r="A27" s="5"/>
       <c r="B27" t="s">
         <v>60</v>
       </c>
@@ -1296,7 +1316,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A28" s="3"/>
+      <c r="A28" s="5"/>
       <c r="B28" t="s">
         <v>61</v>
       </c>
@@ -1311,13 +1331,13 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A29" s="3"/>
+      <c r="A29" s="5"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A30" s="3"/>
+      <c r="A30" s="5"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A31" s="3"/>
+      <c r="A31" s="5"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
@@ -1337,10 +1357,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1354,14 +1374,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
@@ -1384,7 +1404,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -1407,7 +1427,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="3"/>
+      <c r="A4" s="5"/>
       <c r="B4" t="s">
         <v>22</v>
       </c>
@@ -1428,7 +1448,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="3"/>
+      <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>23</v>
       </c>
@@ -1449,7 +1469,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="3"/>
+      <c r="A6" s="5"/>
       <c r="B6" t="s">
         <v>24</v>
       </c>
@@ -1470,7 +1490,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="3"/>
+      <c r="A7" s="5"/>
       <c r="B7" t="s">
         <v>25</v>
       </c>
@@ -1491,7 +1511,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="3"/>
+      <c r="A8" s="5"/>
       <c r="B8" t="s">
         <v>36</v>
       </c>
@@ -1512,7 +1532,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="3"/>
+      <c r="A9" s="5"/>
       <c r="B9" t="s">
         <v>35</v>
       </c>
@@ -1532,23 +1552,23 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="3"/>
-      <c r="B10" s="5" t="s">
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="5"/>
+      <c r="B10" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="3" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B12" t="s">
@@ -1565,7 +1585,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="3"/>
+      <c r="A13" s="5"/>
       <c r="B13" t="s">
         <v>43</v>
       </c>
@@ -1586,7 +1606,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="3"/>
+      <c r="A14" s="5"/>
       <c r="B14" t="s">
         <v>44</v>
       </c>
@@ -1607,7 +1627,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="3"/>
+      <c r="A15" s="5"/>
       <c r="B15" t="s">
         <v>41</v>
       </c>
@@ -1628,7 +1648,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="3"/>
+      <c r="A16" s="5"/>
       <c r="B16" t="s">
         <v>48</v>
       </c>
@@ -1649,7 +1669,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A17" s="3"/>
+      <c r="A17" s="5"/>
       <c r="B17" t="s">
         <v>42</v>
       </c>
@@ -1670,7 +1690,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A18" s="3"/>
+      <c r="A18" s="5"/>
       <c r="B18" t="s">
         <v>49</v>
       </c>
@@ -1691,7 +1711,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A19" s="3"/>
+      <c r="A19" s="5"/>
       <c r="B19" t="s">
         <v>61</v>
       </c>
@@ -1709,7 +1729,7 @@
       <c r="A20" s="2"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B21" t="s">
@@ -1729,167 +1749,185 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A22" s="3"/>
+      <c r="A22" s="5"/>
       <c r="B22" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" t="s">
+        <v>110</v>
+      </c>
+      <c r="G22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A23" s="5"/>
+      <c r="B23" t="s">
         <v>87</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>89</v>
-      </c>
-      <c r="E22" t="s">
-        <v>70</v>
-      </c>
-      <c r="F22" t="s">
-        <v>84</v>
-      </c>
-      <c r="G22" t="s">
-        <v>85</v>
-      </c>
-      <c r="H22" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A23" s="3"/>
-      <c r="B23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C23" t="s">
-        <v>90</v>
       </c>
       <c r="E23" t="s">
         <v>70</v>
       </c>
       <c r="F23" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H23" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A24" s="3"/>
+      <c r="A24" s="5"/>
       <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24" t="s">
+        <v>83</v>
+      </c>
+      <c r="G24" t="s">
+        <v>86</v>
+      </c>
+      <c r="H24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A25" s="5"/>
+      <c r="B25" t="s">
         <v>65</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>66</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>26</v>
       </c>
-      <c r="F24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="F25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G25" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="3"/>
-      <c r="B25" s="6" t="s">
+    <row r="26" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="5"/>
+      <c r="B26" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C26" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F26" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G26" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A26" s="3"/>
-      <c r="B26" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A27" s="5"/>
+      <c r="B27" t="s">
         <v>77</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>79</v>
       </c>
-      <c r="F26" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="F27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A27" s="3"/>
-      <c r="B27" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A28" s="5"/>
+      <c r="B28" t="s">
         <v>78</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>80</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E28" t="s">
         <v>26</v>
       </c>
-      <c r="F27" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="F28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="29" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="30" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A30" s="3"/>
-      <c r="B30" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A31" s="5"/>
+      <c r="B31" t="s">
         <v>59</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>4</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>94</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F31" t="s">
         <v>68</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G31" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A31" s="3"/>
-      <c r="B31" t="s">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A32" s="5"/>
+      <c r="B32" t="s">
         <v>60</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>5</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F32" t="s">
         <v>67</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G32" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A32" s="3"/>
-    </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A33" s="3"/>
+      <c r="A33" s="5"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A34" s="3"/>
+      <c r="A34" s="5"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A35" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="A30:A35"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="A3:A10"/>
-    <mergeCell ref="A21:A27"/>
+    <mergeCell ref="A21:A28"/>
     <mergeCell ref="A12:A19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>